<commit_message>
primer commit del pdfbox por jorge 30-10-2019
</commit_message>
<xml_diff>
--- a/Architecture-analysis-result/issue/arch-issue-cost/ArchIssue-Cost.xlsx
+++ b/Architecture-analysis-result/issue/arch-issue-cost/ArchIssue-Cost.xlsx
@@ -47,16 +47,16 @@
     <t>% Tot Loc changed</t>
   </si>
   <si>
+    <t>PackageCycle</t>
+  </si>
+  <si>
     <t>Clique</t>
   </si>
   <si>
+    <t>Crossing</t>
+  </si>
+  <si>
     <t>UnhealthyInheritance</t>
-  </si>
-  <si>
-    <t>PackageCycle</t>
-  </si>
-  <si>
-    <t>Crossing</t>
   </si>
   <si>
     <t>UnstableInterface</t>
@@ -234,19 +234,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>25.0</v>
+        <v>437.0</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>40.0</v>
+        <v>328.0</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>1629.0</v>
+        <v>6089.0</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>52.0</v>
+        <v>4392.0</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>3458.0</v>
+        <v>190886.0</v>
       </c>
       <c r="G2" s="13">
         <f>B2/B9</f>
@@ -269,19 +269,19 @@
         <v>12</v>
       </c>
       <c r="B3" t="n" s="4">
-        <v>47.0</v>
+        <v>557.0</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>54.0</v>
+        <v>399.0</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>2456.0</v>
+        <v>7451.0</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>77.0</v>
+        <v>5994.0</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>4334.0</v>
+        <v>258196.0</v>
       </c>
       <c r="G3" s="13">
         <f>B3/B9</f>
@@ -304,19 +304,19 @@
         <v>13</v>
       </c>
       <c r="B4" t="n" s="4">
-        <v>59.0</v>
+        <v>626.0</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>58.0</v>
+        <v>489.0</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>2051.0</v>
+        <v>9239.0</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>106.0</v>
+        <v>7409.0</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>5785.0</v>
+        <v>314094.0</v>
       </c>
       <c r="G4" s="13">
         <f>B4/B9</f>
@@ -339,19 +339,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="n" s="4">
-        <v>71.0</v>
+        <v>661.0</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>65.0</v>
+        <v>501.0</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>2201.0</v>
+        <v>10814.0</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>115.0</v>
+        <v>6943.0</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>7033.0</v>
+        <v>299387.0</v>
       </c>
       <c r="G5" s="13">
         <f>B5/B9</f>
@@ -374,19 +374,19 @@
         <v>15</v>
       </c>
       <c r="B6" t="n" s="4">
-        <v>98.0</v>
+        <v>730.0</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>79.0</v>
+        <v>511.0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>2721.0</v>
+        <v>9361.0</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>146.0</v>
+        <v>8126.0</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>7600.0</v>
+        <v>337219.0</v>
       </c>
       <c r="G6" s="13">
         <f>B6/B9</f>
@@ -409,19 +409,19 @@
         <v>16</v>
       </c>
       <c r="B7" t="n" s="4">
-        <v>99.0</v>
+        <v>933.0</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>80.0</v>
+        <v>548.0</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>2830.0</v>
+        <v>10080.0</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>147.0</v>
+        <v>9145.0</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>7600.0</v>
+        <v>379858.0</v>
       </c>
       <c r="G7" s="13">
         <f>B7/B9</f>
@@ -444,19 +444,19 @@
         <v>17</v>
       </c>
       <c r="B9" t="n" s="4">
-        <v>99.0</v>
+        <v>1215.0</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>80.0</v>
+        <v>600.0</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>2830.0</v>
+        <v>13541.0</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>147.0</v>
+        <v>9765.0</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>7600.0</v>
+        <v>406702.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
primer commit del pdfbox por jorge 4-11-2019
</commit_message>
<xml_diff>
--- a/Architecture-analysis-result/issue/arch-issue-cost/ArchIssue-Cost.xlsx
+++ b/Architecture-analysis-result/issue/arch-issue-cost/ArchIssue-Cost.xlsx
@@ -269,19 +269,19 @@
         <v>12</v>
       </c>
       <c r="B3" t="n" s="4">
-        <v>557.0</v>
+        <v>512.0</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>399.0</v>
+        <v>376.0</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>7451.0</v>
+        <v>7095.0</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>5994.0</v>
+        <v>5638.0</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>258196.0</v>
+        <v>243693.0</v>
       </c>
       <c r="G3" s="13">
         <f>B3/B9</f>
@@ -339,7 +339,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="n" s="4">
-        <v>661.0</v>
+        <v>662.0</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>501.0</v>
@@ -348,10 +348,10 @@
         <v>10814.0</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>6943.0</v>
+        <v>6946.0</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>299387.0</v>
+        <v>299584.0</v>
       </c>
       <c r="G5" s="13">
         <f>B5/B9</f>

</xml_diff>